<commit_message>
Updated meeting-notes, documentation, and added POC codebase for Python Flask + Kafka
</commit_message>
<xml_diff>
--- a/Documentation/Microservices-Overview/Project 1- ADS - Design Proposal 1.xlsx
+++ b/Documentation/Microservices-Overview/Project 1- ADS - Design Proposal 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rutja\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Vikrant\GIT_Repos\scapsulators\Documentation\Microservices-Overview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E41B44-299B-41CD-BC84-58C163210136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619C592D-B48F-41D2-B1AB-26B5B6F6A45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Flow Diagram" sheetId="1" r:id="rId1"/>
@@ -409,38 +409,8 @@
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -454,23 +424,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -499,11 +475,35 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1230,6 +1230,19 @@
             </a:rPr>
             <a:t> PAGE</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(includes Audit table)</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1600">
             <a:solidFill>
               <a:schemeClr val="accent1">
@@ -1296,7 +1309,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Search</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3160,15 +3176,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>273050</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:colOff>153308</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>104320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>282702</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>27432</xdr:rowOff>
+      <xdr:colOff>162960</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>125403</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3182,9 +3198,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9417050" y="4425950"/>
-          <a:ext cx="1228852" cy="389382"/>
+        <a:xfrm rot="1610791">
+          <a:off x="9297308" y="4730749"/>
+          <a:ext cx="1228852" cy="391197"/>
         </a:xfrm>
         <a:prstGeom prst="leftRightArrow">
           <a:avLst/>
@@ -4047,322 +4063,322 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:S58"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="4:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="24" t="s">
+    <row r="4" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="26"/>
-    </row>
-    <row r="5" spans="4:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D5" s="27"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="29"/>
-    </row>
-    <row r="6" spans="4:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="30"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="32"/>
-    </row>
-    <row r="7" spans="4:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-    </row>
-    <row r="38" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B38" s="7" t="s">
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="18"/>
+    </row>
+    <row r="5" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="21"/>
+    </row>
+    <row r="6" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="24"/>
+    </row>
+    <row r="7" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="38" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B38" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="7" t="s">
+      <c r="C38" s="27"/>
+      <c r="D38" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B39" s="1"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="15"/>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B40" s="6" t="s">
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B39" s="13"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B40" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="9" t="s">
+      <c r="C40" s="25"/>
+      <c r="D40" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B43" s="1"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="15"/>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B44" s="8" t="s">
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B43" s="13"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B44" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9" t="s">
+      <c r="C44" s="9"/>
+      <c r="D44" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B47" s="1"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="15"/>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B48" s="8" t="s">
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B47" s="13"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B48" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8" t="s">
+      <c r="C48" s="9"/>
+      <c r="D48" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B51" s="1"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="16"/>
-      <c r="I51" s="15"/>
-      <c r="J51" s="12"/>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B52" s="8" t="s">
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B51" s="13"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B52" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="9" t="s">
+      <c r="C52" s="9"/>
+      <c r="D52" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="12"/>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="12"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B56" s="8" t="s">
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="2"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B56" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8" t="s">
+      <c r="C56" s="9"/>
+      <c r="D56" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:C58"/>
-    <mergeCell ref="D56:G58"/>
-    <mergeCell ref="B52:C54"/>
-    <mergeCell ref="D52:G54"/>
+    <mergeCell ref="D4:S6"/>
+    <mergeCell ref="B40:C42"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="D40:G42"/>
     <mergeCell ref="B39:G39"/>
     <mergeCell ref="B43:G43"/>
     <mergeCell ref="B47:G47"/>
@@ -4371,11 +4387,11 @@
     <mergeCell ref="D44:G46"/>
     <mergeCell ref="B48:C50"/>
     <mergeCell ref="D48:G50"/>
-    <mergeCell ref="D4:S6"/>
-    <mergeCell ref="B40:C42"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="D40:G42"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:C58"/>
+    <mergeCell ref="D56:G58"/>
+    <mergeCell ref="B52:C54"/>
+    <mergeCell ref="D52:G54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4387,85 +4403,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1345171C-9A87-4581-B590-A004D669ECB2}">
   <dimension ref="D5:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:Y7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="5" spans="4:25" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D5" s="33" t="s">
+    <row r="5" spans="4:25" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="34"/>
-      <c r="W5" s="34"/>
-      <c r="X5" s="34"/>
-      <c r="Y5" s="34"/>
-    </row>
-    <row r="6" spans="4:25" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="34"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34"/>
-      <c r="U6" s="34"/>
-      <c r="V6" s="34"/>
-      <c r="W6" s="34"/>
-      <c r="X6" s="34"/>
-      <c r="Y6" s="34"/>
-    </row>
-    <row r="7" spans="4:25" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="34"/>
-      <c r="S7" s="34"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="34"/>
-      <c r="V7" s="34"/>
-      <c r="W7" s="34"/>
-      <c r="X7" s="34"/>
-      <c r="Y7" s="34"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="29"/>
+    </row>
+    <row r="6" spans="4:25" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="29"/>
+    </row>
+    <row r="7" spans="4:25" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4481,551 +4497,537 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962FD25A-8621-4291-B91A-4BC1551AF5EB}">
   <dimension ref="C5:L40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="10.26953125" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C5" s="23" t="s">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C5" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-    </row>
-    <row r="9" spans="3:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C9" s="19" t="s">
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+    </row>
+    <row r="9" spans="3:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C9" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19" t="s">
+      <c r="D9" s="34"/>
+      <c r="E9" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19" t="s">
+      <c r="F9" s="34"/>
+      <c r="G9" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19" t="s">
+      <c r="H9" s="34"/>
+      <c r="I9" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19" t="s">
+      <c r="J9" s="34"/>
+      <c r="K9" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="19"/>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C11" s="21" t="s">
+      <c r="L9" s="34"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C11" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C14" s="20">
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C14" s="30">
         <v>1</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20" t="s">
+      <c r="D14" s="30"/>
+      <c r="E14" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C16" s="20">
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="30">
         <v>2</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20" t="s">
+      <c r="D16" s="30"/>
+      <c r="E16" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C18" s="20">
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="30">
         <v>3</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20" t="s">
+      <c r="D18" s="30"/>
+      <c r="E18" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C20" s="20">
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C20" s="30">
         <v>4</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20" t="s">
+      <c r="D20" s="30"/>
+      <c r="E20" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C22" s="20">
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C22" s="30">
         <v>5</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20" t="s">
+      <c r="D22" s="30"/>
+      <c r="E22" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C24" s="22" t="s">
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C24" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-    </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C26" s="20">
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C26" s="30">
         <v>1</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20" t="s">
+      <c r="D26" s="30"/>
+      <c r="E26" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-    </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-    </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C28" s="20">
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C28" s="30">
         <v>2</v>
       </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20" t="s">
+      <c r="D28" s="30"/>
+      <c r="E28" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-    </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-    </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C30" s="20">
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C30" s="30">
         <v>3</v>
       </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20" t="s">
+      <c r="D30" s="30"/>
+      <c r="E30" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-    </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-    </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C32" s="20">
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C32" s="30">
         <v>4</v>
       </c>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20" t="s">
+      <c r="D32" s="30"/>
+      <c r="E32" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-    </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C34" s="20">
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C34" s="30">
         <v>5</v>
       </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20" t="s">
+      <c r="D34" s="30"/>
+      <c r="E34" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-    </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-    </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C36" s="20">
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="30">
         <v>6</v>
       </c>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20" t="s">
+      <c r="D36" s="30"/>
+      <c r="E36" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-    </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C38" s="20">
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="30"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C38" s="30">
         <v>7</v>
       </c>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20" t="s">
+      <c r="D38" s="30"/>
+      <c r="E38" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-    </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-    </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C40" s="20">
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30"/>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C40" s="30">
         <v>8</v>
       </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20" t="s">
+      <c r="D40" s="30"/>
+      <c r="E40" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="C39:L39"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="C37:L37"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="C35:L35"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="C33:L33"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="C31:L31"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="C29:L29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="C10:L10"/>
+    <mergeCell ref="C5:L7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="C11:L12"/>
+    <mergeCell ref="C13:L13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="C17:L17"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="C19:L19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:L20"/>
     <mergeCell ref="C27:L27"/>
     <mergeCell ref="C23:L23"/>
     <mergeCell ref="C24:L25"/>
@@ -5035,38 +5037,52 @@
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="K22:L22"/>
-    <mergeCell ref="C19:L19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="C17:L17"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="C11:L12"/>
-    <mergeCell ref="C13:L13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="C10:L10"/>
-    <mergeCell ref="C5:L7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="C31:L31"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="C29:L29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="C35:L35"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="C33:L33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="C39:L39"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="C37:L37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="K40:L40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Created branches for development and release management
</commit_message>
<xml_diff>
--- a/Documentation/Microservices-Overview/Project 1- ADS - Design Proposal 1.xlsx
+++ b/Documentation/Microservices-Overview/Project 1- ADS - Design Proposal 1.xlsx
@@ -8,26 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Vikrant\GIT_Repos\scapsulators\Documentation\Microservices-Overview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619C592D-B48F-41D2-B1AB-26B5B6F6A45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3149C2-1C72-41AC-B497-A142CB1DD045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Flow Diagram" sheetId="1" r:id="rId1"/>
     <sheet name="Project System Design" sheetId="2" r:id="rId2"/>
     <sheet name="Task Allocation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>LOGIN PAGE</t>
   </si>
@@ -130,22 +139,91 @@
     <t>API GATEWAY</t>
   </si>
   <si>
-    <t xml:space="preserve">SIGN UP </t>
-  </si>
-  <si>
-    <t>AUDIT SAVE</t>
-  </si>
-  <si>
-    <t>AUDIT FETCH</t>
-  </si>
-  <si>
-    <t>NEXRAD DATA FETCH</t>
-  </si>
-  <si>
-    <t>DB CONNECTION</t>
-  </si>
-  <si>
-    <t>AWS CONNECTION</t>
+    <t>Shubham</t>
+  </si>
+  <si>
+    <t>Rutuja</t>
+  </si>
+  <si>
+    <t>Vikrant</t>
+  </si>
+  <si>
+    <t>Rutuja/Vikrant</t>
+  </si>
+  <si>
+    <t>WEATHER REPORTER</t>
+  </si>
+  <si>
+    <t>NEXRAD STATIONS FETCHER</t>
+  </si>
+  <si>
+    <t>Vikrant/Shubham</t>
+  </si>
+  <si>
+    <t>Framework/Language</t>
+  </si>
+  <si>
+    <t>NodeJS</t>
+  </si>
+  <si>
+    <t>Java SpringBoot</t>
+  </si>
+  <si>
+    <t>AUTHENTICATOR (LOGIN/REGISTER)</t>
+  </si>
+  <si>
+    <t>DB CONNECTOR</t>
+  </si>
+  <si>
+    <t>Java SpringBoot w MongoDB</t>
+  </si>
+  <si>
+    <t>Python Flask</t>
+  </si>
+  <si>
+    <t>Python/React</t>
+  </si>
+  <si>
+    <t>React</t>
+  </si>
+  <si>
+    <t>AUDIT SAVE/FETCH</t>
+  </si>
+  <si>
+    <t>FastAPI Python</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>Research persistence in Docker container. Backup is @Override run()</t>
+  </si>
+  <si>
+    <t>Implementing in REST for PROJECT-1. Will be scrapped for PROJECT-2.</t>
+  </si>
+  <si>
+    <t>project1-release</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>development-gateway</t>
+  </si>
+  <si>
+    <t>development-authentication</t>
+  </si>
+  <si>
+    <t>development-audit</t>
+  </si>
+  <si>
+    <t>development-dbconnection</t>
+  </si>
+  <si>
+    <t>development-radarstations</t>
+  </si>
+  <si>
+    <t>development-reportweather</t>
   </si>
 </sst>
 </file>
@@ -407,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -424,30 +502,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -484,25 +538,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4070,60 +4155,60 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="4" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="18"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="10"/>
     </row>
     <row r="5" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="21"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="13"/>
     </row>
     <row r="6" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="24"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="16"/>
     </row>
     <row r="7" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D7" s="1"/>
@@ -4144,242 +4229,241 @@
       <c r="S7" s="1"/>
     </row>
     <row r="38" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="27"/>
-      <c r="D38" s="26" t="s">
+      <c r="C38" s="19"/>
+      <c r="D38" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="13"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="15"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="23"/>
       <c r="H39" s="6"/>
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="11" t="s">
+      <c r="C40" s="17"/>
+      <c r="D40" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="13"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="15"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="23"/>
       <c r="H43" s="6"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="11" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B47" s="13"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="15"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="23"/>
       <c r="H47" s="6"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9" t="s">
+      <c r="C48" s="24"/>
+      <c r="D48" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B51" s="13"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="15"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="23"/>
       <c r="H51" s="6"/>
       <c r="I51" s="5"/>
       <c r="J51" s="2"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="11" t="s">
+      <c r="C52" s="24"/>
+      <c r="D52" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="2"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="2"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9" t="s">
+      <c r="C56" s="24"/>
+      <c r="D56" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D4:S6"/>
-    <mergeCell ref="B40:C42"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="D40:G42"/>
-    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:C58"/>
+    <mergeCell ref="D56:G58"/>
+    <mergeCell ref="B52:C54"/>
+    <mergeCell ref="D52:G54"/>
     <mergeCell ref="B43:G43"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B51:G51"/>
@@ -4387,11 +4471,12 @@
     <mergeCell ref="D44:G46"/>
     <mergeCell ref="B48:C50"/>
     <mergeCell ref="D48:G50"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:C58"/>
-    <mergeCell ref="D56:G58"/>
-    <mergeCell ref="B52:C54"/>
-    <mergeCell ref="D52:G54"/>
+    <mergeCell ref="D4:S6"/>
+    <mergeCell ref="B40:C42"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="D40:G42"/>
+    <mergeCell ref="B39:G39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4403,8 +4488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1345171C-9A87-4581-B590-A004D669ECB2}">
   <dimension ref="D5:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4495,163 +4580,300 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962FD25A-8621-4291-B91A-4BC1551AF5EB}">
-  <dimension ref="C5:L40"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="10.21875" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="35" customWidth="1"/>
+    <col min="4" max="4" width="18" style="35" customWidth="1"/>
+    <col min="5" max="6" width="8.88671875" style="35"/>
+    <col min="7" max="7" width="14.88671875" style="35" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="35" customWidth="1"/>
+    <col min="9" max="12" width="8.88671875" style="35"/>
+    <col min="13" max="13" width="13.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="35"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C5" s="33" t="s">
+    <row r="1" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
     </row>
-    <row r="9" spans="3:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C9" s="34" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34" t="s">
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34" t="s">
+      <c r="F5" s="36"/>
+      <c r="G5" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34" t="s">
+      <c r="J5" s="36"/>
+      <c r="K5" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="34"/>
+      <c r="L5" s="36"/>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C11" s="32" t="s">
+    <row r="7" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
         <v>20</v>
       </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="31">
+        <v>1</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="31"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="31">
+        <v>2</v>
+      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="31">
+        <v>3</v>
+      </c>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31" t="s">
+        <v>8</v>
+      </c>
       <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
+      <c r="E11" s="31" t="s">
+        <v>25</v>
+      </c>
       <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
+      <c r="G11" s="31" t="s">
+        <v>40</v>
+      </c>
       <c r="H11" s="31"/>
       <c r="I11" s="31"/>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C12" s="31"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="31">
+        <v>4</v>
+      </c>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31" t="s">
+        <v>21</v>
+      </c>
       <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
+      <c r="E12" s="31" t="s">
+        <v>25</v>
+      </c>
       <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
+      <c r="G12" s="31" t="s">
+        <v>40</v>
+      </c>
       <c r="H12" s="31"/>
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="31">
+        <v>5</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C14" s="30">
-        <v>1</v>
-      </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C16" s="30">
-        <v>2</v>
-      </c>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="30"/>
-      <c r="E16" s="30" t="s">
-        <v>5</v>
-      </c>
+      <c r="E16" s="30"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
       <c r="H16" s="30"/>
@@ -4660,429 +4882,280 @@
       <c r="K16" s="30"/>
       <c r="L16" s="30"/>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="31">
+        <v>1</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" s="31"/>
+      <c r="M17" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="N17" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="O17" s="35" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C18" s="30">
-        <v>3</v>
-      </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30" t="s">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="31">
+        <v>2</v>
+      </c>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="L18" s="31"/>
+      <c r="M18" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="N18" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="O18" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="31">
+        <v>4</v>
+      </c>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="N19" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="O19" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="31">
+        <v>6</v>
+      </c>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="L20" s="31"/>
+      <c r="M20" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="N20" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="O20" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="31">
+        <v>7</v>
+      </c>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="L21" s="31"/>
+      <c r="M21" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="O21" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="31">
         <v>8</v>
       </c>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C20" s="30">
-        <v>4</v>
-      </c>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C22" s="30">
-        <v>5</v>
-      </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C24" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-    </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C26" s="30">
-        <v>1</v>
-      </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-    </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C28" s="30">
-        <v>2</v>
-      </c>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-    </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-    </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C30" s="30">
-        <v>3</v>
-      </c>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-    </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-    </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C32" s="30">
-        <v>4</v>
-      </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-    </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C34" s="30">
-        <v>5</v>
-      </c>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30" t="s">
+      <c r="B22" s="31"/>
+      <c r="C22" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-    </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-    </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C36" s="30">
-        <v>6</v>
-      </c>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-    </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C38" s="30">
-        <v>7</v>
-      </c>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-    </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-    </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C40" s="30">
-        <v>8</v>
-      </c>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="30"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="N22" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="O22" s="35" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="87">
-    <mergeCell ref="C10:L10"/>
-    <mergeCell ref="C5:L7"/>
+  <mergeCells count="78">
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="A15:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="C11:L12"/>
-    <mergeCell ref="C13:L13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="C17:L17"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="C19:L19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="C27:L27"/>
-    <mergeCell ref="C23:L23"/>
-    <mergeCell ref="C24:L25"/>
-    <mergeCell ref="C21:L21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="C31:L31"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="C29:L29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="C35:L35"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="C33:L33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="C39:L39"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="C37:L37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="A7:L8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feature update for gateway #42
</commit_message>
<xml_diff>
--- a/Documentation/Microservices-Overview/Project 1- ADS - Design Proposal 1.xlsx
+++ b/Documentation/Microservices-Overview/Project 1- ADS - Design Proposal 1.xlsx
@@ -8,35 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Vikrant\GIT_Repos\scapsulators\Documentation\Microservices-Overview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3149C2-1C72-41AC-B497-A142CB1DD045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619C592D-B48F-41D2-B1AB-26B5B6F6A45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Flow Diagram" sheetId="1" r:id="rId1"/>
     <sheet name="Project System Design" sheetId="2" r:id="rId2"/>
     <sheet name="Task Allocation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>LOGIN PAGE</t>
   </si>
@@ -139,91 +130,22 @@
     <t>API GATEWAY</t>
   </si>
   <si>
-    <t>Shubham</t>
+    <t xml:space="preserve">SIGN UP </t>
   </si>
   <si>
-    <t>Rutuja</t>
+    <t>AUDIT SAVE</t>
   </si>
   <si>
-    <t>Vikrant</t>
+    <t>AUDIT FETCH</t>
   </si>
   <si>
-    <t>Rutuja/Vikrant</t>
+    <t>NEXRAD DATA FETCH</t>
   </si>
   <si>
-    <t>WEATHER REPORTER</t>
+    <t>DB CONNECTION</t>
   </si>
   <si>
-    <t>NEXRAD STATIONS FETCHER</t>
-  </si>
-  <si>
-    <t>Vikrant/Shubham</t>
-  </si>
-  <si>
-    <t>Framework/Language</t>
-  </si>
-  <si>
-    <t>NodeJS</t>
-  </si>
-  <si>
-    <t>Java SpringBoot</t>
-  </si>
-  <si>
-    <t>AUTHENTICATOR (LOGIN/REGISTER)</t>
-  </si>
-  <si>
-    <t>DB CONNECTOR</t>
-  </si>
-  <si>
-    <t>Java SpringBoot w MongoDB</t>
-  </si>
-  <si>
-    <t>Python Flask</t>
-  </si>
-  <si>
-    <t>Python/React</t>
-  </si>
-  <si>
-    <t>React</t>
-  </si>
-  <si>
-    <t>AUDIT SAVE/FETCH</t>
-  </si>
-  <si>
-    <t>FastAPI Python</t>
-  </si>
-  <si>
-    <t>Optional</t>
-  </si>
-  <si>
-    <t>Research persistence in Docker container. Backup is @Override run()</t>
-  </si>
-  <si>
-    <t>Implementing in REST for PROJECT-1. Will be scrapped for PROJECT-2.</t>
-  </si>
-  <si>
-    <t>project1-release</t>
-  </si>
-  <si>
-    <t>main</t>
-  </si>
-  <si>
-    <t>development-gateway</t>
-  </si>
-  <si>
-    <t>development-authentication</t>
-  </si>
-  <si>
-    <t>development-audit</t>
-  </si>
-  <si>
-    <t>development-dbconnection</t>
-  </si>
-  <si>
-    <t>development-radarstations</t>
-  </si>
-  <si>
-    <t>development-reportweather</t>
+    <t>AWS CONNECTION</t>
   </si>
 </sst>
 </file>
@@ -485,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -502,6 +424,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -538,56 +484,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4155,60 +4070,60 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="4" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="10"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="18"/>
     </row>
     <row r="5" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="13"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="21"/>
     </row>
     <row r="6" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="16"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="24"/>
     </row>
     <row r="7" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D7" s="1"/>
@@ -4229,241 +4144,242 @@
       <c r="S7" s="1"/>
     </row>
     <row r="38" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="18" t="s">
+      <c r="C38" s="27"/>
+      <c r="D38" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="21"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="23"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="15"/>
       <c r="H39" s="6"/>
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="20" t="s">
+      <c r="C40" s="25"/>
+      <c r="D40" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="21"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="23"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="15"/>
       <c r="H43" s="6"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="20" t="s">
+      <c r="C44" s="9"/>
+      <c r="D44" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B47" s="21"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="23"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="15"/>
       <c r="H47" s="6"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B48" s="24" t="s">
+      <c r="B48" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24" t="s">
+      <c r="C48" s="9"/>
+      <c r="D48" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B51" s="21"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="23"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="15"/>
       <c r="H51" s="6"/>
       <c r="I51" s="5"/>
       <c r="J51" s="2"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C52" s="24"/>
-      <c r="D52" s="20" t="s">
+      <c r="C52" s="9"/>
+      <c r="D52" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="2"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="2"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="27"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B56" s="24" t="s">
+      <c r="B56" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="24"/>
-      <c r="D56" s="24" t="s">
+      <c r="C56" s="9"/>
+      <c r="D56" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="24"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B58" s="24"/>
-      <c r="C58" s="24"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:C58"/>
-    <mergeCell ref="D56:G58"/>
-    <mergeCell ref="B52:C54"/>
-    <mergeCell ref="D52:G54"/>
+    <mergeCell ref="D4:S6"/>
+    <mergeCell ref="B40:C42"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="D40:G42"/>
+    <mergeCell ref="B39:G39"/>
     <mergeCell ref="B43:G43"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B51:G51"/>
@@ -4471,12 +4387,11 @@
     <mergeCell ref="D44:G46"/>
     <mergeCell ref="B48:C50"/>
     <mergeCell ref="D48:G50"/>
-    <mergeCell ref="D4:S6"/>
-    <mergeCell ref="B40:C42"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="D40:G42"/>
-    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:C58"/>
+    <mergeCell ref="D56:G58"/>
+    <mergeCell ref="B52:C54"/>
+    <mergeCell ref="D52:G54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4488,8 +4403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1345171C-9A87-4581-B590-A004D669ECB2}">
   <dimension ref="D5:Y7"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4580,300 +4495,163 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962FD25A-8621-4291-B91A-4BC1551AF5EB}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="C5:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="35" customWidth="1"/>
-    <col min="4" max="4" width="18" style="35" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" style="35"/>
-    <col min="7" max="7" width="14.88671875" style="35" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" style="35" customWidth="1"/>
-    <col min="9" max="12" width="8.88671875" style="35"/>
-    <col min="13" max="13" width="13.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="35"/>
+    <col min="6" max="6" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C5" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+    </row>
+    <row r="9" spans="3:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C9" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36" t="s">
+      <c r="D9" s="34"/>
+      <c r="E9" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36" t="s">
+      <c r="F9" s="34"/>
+      <c r="G9" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36" t="s">
+      <c r="H9" s="34"/>
+      <c r="I9" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36" t="s">
+      <c r="J9" s="34"/>
+      <c r="K9" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="36"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-    </row>
-    <row r="7" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
+      <c r="L9" s="34"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C11" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="31">
-        <v>1</v>
-      </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="31"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="31">
-        <v>2</v>
-      </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="31">
-        <v>3</v>
-      </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31" t="s">
-        <v>8</v>
-      </c>
       <c r="D11" s="31"/>
-      <c r="E11" s="31" t="s">
-        <v>25</v>
-      </c>
+      <c r="E11" s="31"/>
       <c r="F11" s="31"/>
-      <c r="G11" s="31" t="s">
-        <v>40</v>
-      </c>
+      <c r="G11" s="31"/>
       <c r="H11" s="31"/>
       <c r="I11" s="31"/>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="31">
-        <v>4</v>
-      </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31" t="s">
-        <v>21</v>
-      </c>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C12" s="31"/>
       <c r="D12" s="31"/>
-      <c r="E12" s="31" t="s">
-        <v>25</v>
-      </c>
+      <c r="E12" s="31"/>
       <c r="F12" s="31"/>
-      <c r="G12" s="31" t="s">
-        <v>40</v>
-      </c>
+      <c r="G12" s="31"/>
       <c r="H12" s="31"/>
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="31">
+    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C14" s="30">
+        <v>1</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="30">
+        <v>2</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
       <c r="H16" s="30"/>
@@ -4882,280 +4660,429 @@
       <c r="K16" s="30"/>
       <c r="L16" s="30"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="31">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="30">
+        <v>3</v>
+      </c>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C20" s="30">
+        <v>4</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C22" s="30">
+        <v>5</v>
+      </c>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C24" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C26" s="30">
         <v>1</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31" t="s">
+      <c r="D26" s="30"/>
+      <c r="E26" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31" t="s">
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C28" s="30">
+        <v>2</v>
+      </c>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C30" s="30">
+        <v>3</v>
+      </c>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31" t="s">
-        <v>33</v>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C32" s="30">
+        <v>4</v>
       </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="L17" s="31"/>
-      <c r="M17" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="N17" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="O17" s="35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="31">
-        <v>2</v>
-      </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31" t="s">
+      <c r="D32" s="30"/>
+      <c r="E32" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31" t="s">
-        <v>34</v>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C34" s="30">
+        <v>5</v>
       </c>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31" t="s">
-        <v>45</v>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30" t="s">
+        <v>27</v>
       </c>
-      <c r="L18" s="31"/>
-      <c r="M18" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N18" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="O18" s="35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="31">
-        <v>4</v>
-      </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="N19" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="O19" s="35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="31">
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="30">
         <v>6</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31" t="s">
+      <c r="D36" s="30"/>
+      <c r="E36" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="L20" s="31"/>
-      <c r="M20" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="N20" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="O20" s="35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="31">
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="30"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C38" s="30">
         <v>7</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31" t="s">
+      <c r="D38" s="30"/>
+      <c r="E38" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30"/>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C40" s="30">
+        <v>8</v>
+      </c>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="L21" s="31"/>
-      <c r="M21" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="N21" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="O21" s="35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="31">
-        <v>8</v>
-      </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="N22" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="O22" s="35" t="s">
-        <v>47</v>
-      </c>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="78">
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="A1:L3"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A6:L6"/>
+  <mergeCells count="87">
+    <mergeCell ref="C10:L10"/>
+    <mergeCell ref="C5:L7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
     <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="C11:L12"/>
+    <mergeCell ref="C13:L13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="C17:L17"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
     <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="C19:L19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
     <mergeCell ref="K20:L20"/>
-    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C27:L27"/>
+    <mergeCell ref="C23:L23"/>
+    <mergeCell ref="C24:L25"/>
+    <mergeCell ref="C21:L21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="A15:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A7:L8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="C31:L31"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="C29:L29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="C35:L35"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="C33:L33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="C39:L39"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="C37:L37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="K40:L40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding frontend feature branch #42
</commit_message>
<xml_diff>
--- a/Documentation/Microservices-Overview/Project 1- ADS - Design Proposal 1.xlsx
+++ b/Documentation/Microservices-Overview/Project 1- ADS - Design Proposal 1.xlsx
@@ -8,26 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Vikrant\GIT_Repos\scapsulators\Documentation\Microservices-Overview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619C592D-B48F-41D2-B1AB-26B5B6F6A45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3149C2-1C72-41AC-B497-A142CB1DD045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Flow Diagram" sheetId="1" r:id="rId1"/>
     <sheet name="Project System Design" sheetId="2" r:id="rId2"/>
     <sheet name="Task Allocation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>LOGIN PAGE</t>
   </si>
@@ -130,22 +139,91 @@
     <t>API GATEWAY</t>
   </si>
   <si>
-    <t xml:space="preserve">SIGN UP </t>
-  </si>
-  <si>
-    <t>AUDIT SAVE</t>
-  </si>
-  <si>
-    <t>AUDIT FETCH</t>
-  </si>
-  <si>
-    <t>NEXRAD DATA FETCH</t>
-  </si>
-  <si>
-    <t>DB CONNECTION</t>
-  </si>
-  <si>
-    <t>AWS CONNECTION</t>
+    <t>Shubham</t>
+  </si>
+  <si>
+    <t>Rutuja</t>
+  </si>
+  <si>
+    <t>Vikrant</t>
+  </si>
+  <si>
+    <t>Rutuja/Vikrant</t>
+  </si>
+  <si>
+    <t>WEATHER REPORTER</t>
+  </si>
+  <si>
+    <t>NEXRAD STATIONS FETCHER</t>
+  </si>
+  <si>
+    <t>Vikrant/Shubham</t>
+  </si>
+  <si>
+    <t>Framework/Language</t>
+  </si>
+  <si>
+    <t>NodeJS</t>
+  </si>
+  <si>
+    <t>Java SpringBoot</t>
+  </si>
+  <si>
+    <t>AUTHENTICATOR (LOGIN/REGISTER)</t>
+  </si>
+  <si>
+    <t>DB CONNECTOR</t>
+  </si>
+  <si>
+    <t>Java SpringBoot w MongoDB</t>
+  </si>
+  <si>
+    <t>Python Flask</t>
+  </si>
+  <si>
+    <t>Python/React</t>
+  </si>
+  <si>
+    <t>React</t>
+  </si>
+  <si>
+    <t>AUDIT SAVE/FETCH</t>
+  </si>
+  <si>
+    <t>FastAPI Python</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>Research persistence in Docker container. Backup is @Override run()</t>
+  </si>
+  <si>
+    <t>Implementing in REST for PROJECT-1. Will be scrapped for PROJECT-2.</t>
+  </si>
+  <si>
+    <t>project1-release</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>development-gateway</t>
+  </si>
+  <si>
+    <t>development-authentication</t>
+  </si>
+  <si>
+    <t>development-audit</t>
+  </si>
+  <si>
+    <t>development-dbconnection</t>
+  </si>
+  <si>
+    <t>development-radarstations</t>
+  </si>
+  <si>
+    <t>development-reportweather</t>
   </si>
 </sst>
 </file>
@@ -407,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -424,30 +502,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -484,25 +538,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4070,60 +4155,60 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="4" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="18"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="10"/>
     </row>
     <row r="5" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="21"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="13"/>
     </row>
     <row r="6" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="24"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="16"/>
     </row>
     <row r="7" spans="4:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D7" s="1"/>
@@ -4144,242 +4229,241 @@
       <c r="S7" s="1"/>
     </row>
     <row r="38" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="27"/>
-      <c r="D38" s="26" t="s">
+      <c r="C38" s="19"/>
+      <c r="D38" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="13"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="15"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="23"/>
       <c r="H39" s="6"/>
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="11" t="s">
+      <c r="C40" s="17"/>
+      <c r="D40" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="13"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="15"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="23"/>
       <c r="H43" s="6"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="11" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B47" s="13"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="15"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="23"/>
       <c r="H47" s="6"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9" t="s">
+      <c r="C48" s="24"/>
+      <c r="D48" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B51" s="13"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="15"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="23"/>
       <c r="H51" s="6"/>
       <c r="I51" s="5"/>
       <c r="J51" s="2"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="11" t="s">
+      <c r="C52" s="24"/>
+      <c r="D52" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="2"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="2"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9" t="s">
+      <c r="C56" s="24"/>
+      <c r="D56" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D4:S6"/>
-    <mergeCell ref="B40:C42"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="D40:G42"/>
-    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:C58"/>
+    <mergeCell ref="D56:G58"/>
+    <mergeCell ref="B52:C54"/>
+    <mergeCell ref="D52:G54"/>
     <mergeCell ref="B43:G43"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B51:G51"/>
@@ -4387,11 +4471,12 @@
     <mergeCell ref="D44:G46"/>
     <mergeCell ref="B48:C50"/>
     <mergeCell ref="D48:G50"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:C58"/>
-    <mergeCell ref="D56:G58"/>
-    <mergeCell ref="B52:C54"/>
-    <mergeCell ref="D52:G54"/>
+    <mergeCell ref="D4:S6"/>
+    <mergeCell ref="B40:C42"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="D40:G42"/>
+    <mergeCell ref="B39:G39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4403,8 +4488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1345171C-9A87-4581-B590-A004D669ECB2}">
   <dimension ref="D5:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4495,163 +4580,300 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962FD25A-8621-4291-B91A-4BC1551AF5EB}">
-  <dimension ref="C5:L40"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="10.21875" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="35" customWidth="1"/>
+    <col min="4" max="4" width="18" style="35" customWidth="1"/>
+    <col min="5" max="6" width="8.88671875" style="35"/>
+    <col min="7" max="7" width="14.88671875" style="35" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="35" customWidth="1"/>
+    <col min="9" max="12" width="8.88671875" style="35"/>
+    <col min="13" max="13" width="13.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="35"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C5" s="33" t="s">
+    <row r="1" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
     </row>
-    <row r="9" spans="3:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C9" s="34" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34" t="s">
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34" t="s">
+      <c r="F5" s="36"/>
+      <c r="G5" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34" t="s">
+      <c r="J5" s="36"/>
+      <c r="K5" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="34"/>
+      <c r="L5" s="36"/>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C11" s="32" t="s">
+    <row r="7" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
         <v>20</v>
       </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="31">
+        <v>1</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="31"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="31">
+        <v>2</v>
+      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="31">
+        <v>3</v>
+      </c>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31" t="s">
+        <v>8</v>
+      </c>
       <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
+      <c r="E11" s="31" t="s">
+        <v>25</v>
+      </c>
       <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
+      <c r="G11" s="31" t="s">
+        <v>40</v>
+      </c>
       <c r="H11" s="31"/>
       <c r="I11" s="31"/>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C12" s="31"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="31">
+        <v>4</v>
+      </c>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31" t="s">
+        <v>21</v>
+      </c>
       <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
+      <c r="E12" s="31" t="s">
+        <v>25</v>
+      </c>
       <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
+      <c r="G12" s="31" t="s">
+        <v>40</v>
+      </c>
       <c r="H12" s="31"/>
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="31">
+        <v>5</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C14" s="30">
-        <v>1</v>
-      </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C16" s="30">
-        <v>2</v>
-      </c>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="30"/>
-      <c r="E16" s="30" t="s">
-        <v>5</v>
-      </c>
+      <c r="E16" s="30"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
       <c r="H16" s="30"/>
@@ -4660,429 +4882,280 @@
       <c r="K16" s="30"/>
       <c r="L16" s="30"/>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="31">
+        <v>1</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" s="31"/>
+      <c r="M17" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="N17" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="O17" s="35" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C18" s="30">
-        <v>3</v>
-      </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30" t="s">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="31">
+        <v>2</v>
+      </c>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="L18" s="31"/>
+      <c r="M18" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="N18" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="O18" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="31">
+        <v>4</v>
+      </c>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="N19" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="O19" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="31">
+        <v>6</v>
+      </c>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="L20" s="31"/>
+      <c r="M20" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="N20" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="O20" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="31">
+        <v>7</v>
+      </c>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="L21" s="31"/>
+      <c r="M21" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="O21" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="31">
         <v>8</v>
       </c>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C20" s="30">
-        <v>4</v>
-      </c>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C22" s="30">
-        <v>5</v>
-      </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C24" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-    </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C26" s="30">
-        <v>1</v>
-      </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-    </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C28" s="30">
-        <v>2</v>
-      </c>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-    </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-    </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C30" s="30">
-        <v>3</v>
-      </c>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-    </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-    </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C32" s="30">
-        <v>4</v>
-      </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-    </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C34" s="30">
-        <v>5</v>
-      </c>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30" t="s">
+      <c r="B22" s="31"/>
+      <c r="C22" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-    </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-    </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C36" s="30">
-        <v>6</v>
-      </c>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-    </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C38" s="30">
-        <v>7</v>
-      </c>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-    </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-    </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C40" s="30">
-        <v>8</v>
-      </c>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="30"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="N22" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="O22" s="35" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="87">
-    <mergeCell ref="C10:L10"/>
-    <mergeCell ref="C5:L7"/>
+  <mergeCells count="78">
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="A15:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="C11:L12"/>
-    <mergeCell ref="C13:L13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="C17:L17"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="C19:L19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="C27:L27"/>
-    <mergeCell ref="C23:L23"/>
-    <mergeCell ref="C24:L25"/>
-    <mergeCell ref="C21:L21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="C31:L31"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="C29:L29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="C35:L35"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="C33:L33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="C39:L39"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="C37:L37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="A7:L8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>